<commit_message>
update with km conversion
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">results!$A$1:$DA$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">results!$A$1:$DA$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
   <si>
     <t xml:space="preserve">algorithm</t>
   </si>
@@ -375,6 +376,9 @@
     <t xml:space="preserve">UnlimitedGreedy</t>
   </si>
   <si>
+    <t xml:space="preserve">steps in px, see fov/slope</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slope 8</t>
   </si>
   <si>
@@ -393,6 +397,9 @@
     <t xml:space="preserve">Slope 18</t>
   </si>
   <si>
+    <t xml:space="preserve">for km conversion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fov 10</t>
   </si>
   <si>
@@ -426,7 +433,7 @@
     <t xml:space="preserve">Slope 32</t>
   </si>
   <si>
-    <t xml:space="preserve">STEPS</t>
+    <t xml:space="preserve">STEPS (in km)</t>
   </si>
   <si>
     <t xml:space="preserve">Diff 17</t>
@@ -438,16 +445,16 @@
     <t xml:space="preserve">Diff 31</t>
   </si>
   <si>
-    <t xml:space="preserve">TIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steps</t>
+    <t xml:space="preserve">TIME (in ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steps (in km)</t>
   </si>
   <si>
     <t xml:space="preserve">time</t>
   </si>
   <si>
-    <t xml:space="preserve">steps/ms</t>
+    <t xml:space="preserve">steps/ms (aka km/ms)</t>
   </si>
 </sst>
 </file>
@@ -835,28 +842,28 @@
   <dimension ref="A1:DA11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6261261261261"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.9234234234234"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4009009009009"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.9234234234234"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5045045045045"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8063063063063"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.2792792792793"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.8063063063063"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1891891891892"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.8288288288288"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.1891891891892"/>
@@ -1899,7 +1906,7 @@
         <v>45829</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>107</v>
       </c>
@@ -4191,126 +4198,132 @@
   </sheetPr>
   <dimension ref="A1:Y41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8828828828829"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.58108108108108"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>115</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>122</v>
+      </c>
       <c r="B2" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="H2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="L2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="O2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="P2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="T2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="W2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="X2" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5437,37 +5450,37 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="S15" s="16"/>
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
       <c r="V15" s="17" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="W15" s="17"/>
       <c r="X15" s="17"/>
@@ -5475,76 +5488,76 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="H16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="L16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="O16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="N16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="P16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="R16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="S16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="R16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="S16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="T16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="W16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="V16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="W16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="X16" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6671,7 +6684,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -6679,16 +6692,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6957,43 +6970,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9234234234234"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8063063063063"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.58108108108108"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
@@ -7001,76 +7014,76 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="H2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="L2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="O2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="P2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="T2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="W2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="X2" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8197,37 +8210,37 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="S15" s="16"/>
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
       <c r="V15" s="17" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="W15" s="17"/>
       <c r="X15" s="17"/>
@@ -8235,76 +8248,76 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="H16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="L16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="O16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="N16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="P16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="R16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="S16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="R16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="S16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="T16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="W16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="V16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="W16" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="X16" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9431,7 +9444,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -9439,16 +9452,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9712,197 +9725,197 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9234234234234"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8063063063063"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.58108108108108"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">results!A2</f>
         <v>LimitedAStar</v>
       </c>
       <c r="B2" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B3,'Steps Overview'!F3,'Steps Overview'!J3,'Steps Overview'!N3,'Steps Overview'!R3,'Steps Overview'!V3,'Steps Overview'!B17,'Steps Overview'!F17,'Steps Overview'!J17,'Steps Overview'!N17,'Steps Overview'!R17,'Steps Overview'!V17,'Steps Overview'!B31)</f>
-        <v>609.461538461538</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B3,'Steps Overview'!F3,'Steps Overview'!J3,'Steps Overview'!N3,'Steps Overview'!R3,'Steps Overview'!V3,'Steps Overview'!B17,'Steps Overview'!F17,'Steps Overview'!J17,'Steps Overview'!N17,'Steps Overview'!R17,'Steps Overview'!V17,'Steps Overview'!B31)</f>
+        <v>140.785615384615</v>
       </c>
       <c r="C2" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!C3,'Steps Overview'!G3,'Steps Overview'!K3,'Steps Overview'!O3,'Steps Overview'!S3,'Steps Overview'!W3,'Steps Overview'!C17,'Steps Overview'!G17,'Steps Overview'!K17,'Steps Overview'!O17,'Steps Overview'!S17,'Steps Overview'!W17,'Steps Overview'!C31)</f>
-        <v>495.461538461538</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!C3,'Steps Overview'!G3,'Steps Overview'!K3,'Steps Overview'!O3,'Steps Overview'!S3,'Steps Overview'!W3,'Steps Overview'!C17,'Steps Overview'!G17,'Steps Overview'!K17,'Steps Overview'!O17,'Steps Overview'!S17,'Steps Overview'!W17,'Steps Overview'!C31)</f>
+        <v>114.451615384615</v>
       </c>
       <c r="D2" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!D3,'Steps Overview'!H3,'Steps Overview'!L3,'Steps Overview'!P3,'Steps Overview'!T3,'Steps Overview'!X3,'Steps Overview'!D17,'Steps Overview'!H17,'Steps Overview'!L17,'Steps Overview'!P17,'Steps Overview'!T17,'Steps Overview'!X17,'Steps Overview'!D31)</f>
-        <v>478.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!D3,'Steps Overview'!H3,'Steps Overview'!L3,'Steps Overview'!P3,'Steps Overview'!T3,'Steps Overview'!X3,'Steps Overview'!D17,'Steps Overview'!H17,'Steps Overview'!L17,'Steps Overview'!P17,'Steps Overview'!T17,'Steps Overview'!X17,'Steps Overview'!D31)</f>
+        <v>110.577923076923</v>
       </c>
       <c r="E2" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!E3,'Steps Overview'!I3,'Steps Overview'!M3,'Steps Overview'!Q3,'Steps Overview'!U3,'Steps Overview'!Y3,'Steps Overview'!E17,'Steps Overview'!I17,'Steps Overview'!M17,'Steps Overview'!Q17,'Steps Overview'!U17,'Steps Overview'!Y17,'Steps Overview'!E31)</f>
-        <v>450.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!E3,'Steps Overview'!I3,'Steps Overview'!M3,'Steps Overview'!Q3,'Steps Overview'!U3,'Steps Overview'!Y3,'Steps Overview'!E17,'Steps Overview'!I17,'Steps Overview'!M17,'Steps Overview'!Q17,'Steps Overview'!U17,'Steps Overview'!Y17,'Steps Overview'!E31)</f>
+        <v>104.109923076923</v>
       </c>
       <c r="F2" s="21" t="n">
         <f aca="false">C2-B2</f>
-        <v>-114</v>
+        <v>-26.334</v>
       </c>
       <c r="G2" s="21" t="n">
         <f aca="false">D2-C2</f>
-        <v>-16.7692307692308</v>
+        <v>-3.87369230769231</v>
       </c>
       <c r="H2" s="21" t="n">
         <f aca="false">E2-D2</f>
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-6.468</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">results!A3</f>
         <v>LimitedBestFirst</v>
       </c>
       <c r="B3" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B4,'Steps Overview'!F4,'Steps Overview'!J4,'Steps Overview'!N4,'Steps Overview'!R4,'Steps Overview'!V4,'Steps Overview'!B18,'Steps Overview'!F18,'Steps Overview'!J18,'Steps Overview'!N18,'Steps Overview'!R18,'Steps Overview'!V18,'Steps Overview'!B32)</f>
-        <v>684.538461538462</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B4,'Steps Overview'!F4,'Steps Overview'!J4,'Steps Overview'!N4,'Steps Overview'!R4,'Steps Overview'!V4,'Steps Overview'!B18,'Steps Overview'!F18,'Steps Overview'!J18,'Steps Overview'!N18,'Steps Overview'!R18,'Steps Overview'!V18,'Steps Overview'!B32)</f>
+        <v>158.128384615385</v>
       </c>
       <c r="C3" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!C4,'Steps Overview'!G4,'Steps Overview'!K4,'Steps Overview'!O4,'Steps Overview'!S4,'Steps Overview'!W4,'Steps Overview'!C18,'Steps Overview'!G18,'Steps Overview'!K18,'Steps Overview'!O18,'Steps Overview'!S18,'Steps Overview'!W18,'Steps Overview'!C32)</f>
-        <v>560.153846153846</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!C4,'Steps Overview'!G4,'Steps Overview'!K4,'Steps Overview'!O4,'Steps Overview'!S4,'Steps Overview'!W4,'Steps Overview'!C18,'Steps Overview'!G18,'Steps Overview'!K18,'Steps Overview'!O18,'Steps Overview'!S18,'Steps Overview'!W18,'Steps Overview'!C32)</f>
+        <v>129.395538461538</v>
       </c>
       <c r="D3" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!D4,'Steps Overview'!H4,'Steps Overview'!L4,'Steps Overview'!P4,'Steps Overview'!T4,'Steps Overview'!X4,'Steps Overview'!D18,'Steps Overview'!H18,'Steps Overview'!L18,'Steps Overview'!P18,'Steps Overview'!T18,'Steps Overview'!X18,'Steps Overview'!D32)</f>
-        <v>537</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!D4,'Steps Overview'!H4,'Steps Overview'!L4,'Steps Overview'!P4,'Steps Overview'!T4,'Steps Overview'!X4,'Steps Overview'!D18,'Steps Overview'!H18,'Steps Overview'!L18,'Steps Overview'!P18,'Steps Overview'!T18,'Steps Overview'!X18,'Steps Overview'!D32)</f>
+        <v>124.047</v>
       </c>
       <c r="E3" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!E4,'Steps Overview'!I4,'Steps Overview'!M4,'Steps Overview'!Q4,'Steps Overview'!U4,'Steps Overview'!Y4,'Steps Overview'!E18,'Steps Overview'!I18,'Steps Overview'!M18,'Steps Overview'!Q18,'Steps Overview'!U18,'Steps Overview'!Y18,'Steps Overview'!E32)</f>
-        <v>511</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!E4,'Steps Overview'!I4,'Steps Overview'!M4,'Steps Overview'!Q4,'Steps Overview'!U4,'Steps Overview'!Y4,'Steps Overview'!E18,'Steps Overview'!I18,'Steps Overview'!M18,'Steps Overview'!Q18,'Steps Overview'!U18,'Steps Overview'!Y18,'Steps Overview'!E32)</f>
+        <v>118.041</v>
       </c>
       <c r="F3" s="21" t="n">
         <f aca="false">C3-B3</f>
-        <v>-124.384615384615</v>
+        <v>-28.7328461538461</v>
       </c>
       <c r="G3" s="21" t="n">
         <f aca="false">D3-C3</f>
-        <v>-23.1538461538462</v>
+        <v>-5.34853846153847</v>
       </c>
       <c r="H3" s="21" t="n">
         <f aca="false">E3-D3</f>
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-6.006</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">results!A4</f>
         <v>LimitedBreadthFirstSearch</v>
       </c>
       <c r="B4" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B5,'Steps Overview'!F5,'Steps Overview'!J5,'Steps Overview'!N5,'Steps Overview'!R5,'Steps Overview'!V5,'Steps Overview'!B19,'Steps Overview'!F19,'Steps Overview'!J19,'Steps Overview'!N19,'Steps Overview'!R19,'Steps Overview'!V19,'Steps Overview'!B33)</f>
-        <v>602.153846153846</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B5,'Steps Overview'!F5,'Steps Overview'!J5,'Steps Overview'!N5,'Steps Overview'!R5,'Steps Overview'!V5,'Steps Overview'!B19,'Steps Overview'!F19,'Steps Overview'!J19,'Steps Overview'!N19,'Steps Overview'!R19,'Steps Overview'!V19,'Steps Overview'!B33)</f>
+        <v>139.097538461538</v>
       </c>
       <c r="C4" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!C5,'Steps Overview'!G5,'Steps Overview'!K5,'Steps Overview'!O5,'Steps Overview'!S5,'Steps Overview'!W5,'Steps Overview'!C19,'Steps Overview'!G19,'Steps Overview'!K19,'Steps Overview'!O19,'Steps Overview'!S19,'Steps Overview'!W19,'Steps Overview'!C33)</f>
-        <v>472.846153846154</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!C5,'Steps Overview'!G5,'Steps Overview'!K5,'Steps Overview'!O5,'Steps Overview'!S5,'Steps Overview'!W5,'Steps Overview'!C19,'Steps Overview'!G19,'Steps Overview'!K19,'Steps Overview'!O19,'Steps Overview'!S19,'Steps Overview'!W19,'Steps Overview'!C33)</f>
+        <v>109.227461538462</v>
       </c>
       <c r="D4" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!D5,'Steps Overview'!H5,'Steps Overview'!L5,'Steps Overview'!P5,'Steps Overview'!T5,'Steps Overview'!X5,'Steps Overview'!D19,'Steps Overview'!H19,'Steps Overview'!L19,'Steps Overview'!P19,'Steps Overview'!T19,'Steps Overview'!X19,'Steps Overview'!D33)</f>
-        <v>455.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!D5,'Steps Overview'!H5,'Steps Overview'!L5,'Steps Overview'!P5,'Steps Overview'!T5,'Steps Overview'!X5,'Steps Overview'!D19,'Steps Overview'!H19,'Steps Overview'!L19,'Steps Overview'!P19,'Steps Overview'!T19,'Steps Overview'!X19,'Steps Overview'!D33)</f>
+        <v>105.264923076923</v>
       </c>
       <c r="E4" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!E5,'Steps Overview'!I5,'Steps Overview'!M5,'Steps Overview'!Q5,'Steps Overview'!U5,'Steps Overview'!Y5,'Steps Overview'!E19,'Steps Overview'!I19,'Steps Overview'!M19,'Steps Overview'!Q19,'Steps Overview'!U19,'Steps Overview'!Y19,'Steps Overview'!E33)</f>
-        <v>466.538461538462</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!E5,'Steps Overview'!I5,'Steps Overview'!M5,'Steps Overview'!Q5,'Steps Overview'!U5,'Steps Overview'!Y5,'Steps Overview'!E19,'Steps Overview'!I19,'Steps Overview'!M19,'Steps Overview'!Q19,'Steps Overview'!U19,'Steps Overview'!Y19,'Steps Overview'!E33)</f>
+        <v>107.770384615385</v>
       </c>
       <c r="F4" s="21" t="n">
         <f aca="false">C4-B4</f>
-        <v>-129.307692307692</v>
+        <v>-29.8700769230769</v>
       </c>
       <c r="G4" s="21" t="n">
         <f aca="false">D4-C4</f>
-        <v>-17.1538461538462</v>
+        <v>-3.96253846153847</v>
       </c>
       <c r="H4" s="21" t="n">
         <f aca="false">E4-D4</f>
-        <v>10.8461538461539</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2.50546153846155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
         <f aca="false">results!A5</f>
         <v>LimitedDijkstra</v>
       </c>
       <c r="B5" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B6,'Steps Overview'!F6,'Steps Overview'!J6,'Steps Overview'!N6,'Steps Overview'!R6,'Steps Overview'!V6,'Steps Overview'!B20,'Steps Overview'!F20,'Steps Overview'!J20,'Steps Overview'!N20,'Steps Overview'!R20,'Steps Overview'!V20,'Steps Overview'!B34)</f>
-        <v>691.153846153846</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B6,'Steps Overview'!F6,'Steps Overview'!J6,'Steps Overview'!N6,'Steps Overview'!R6,'Steps Overview'!V6,'Steps Overview'!B20,'Steps Overview'!F20,'Steps Overview'!J20,'Steps Overview'!N20,'Steps Overview'!R20,'Steps Overview'!V20,'Steps Overview'!B34)</f>
+        <v>159.656538461538</v>
       </c>
       <c r="C5" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!C6,'Steps Overview'!G6,'Steps Overview'!K6,'Steps Overview'!O6,'Steps Overview'!S6,'Steps Overview'!W6,'Steps Overview'!C20,'Steps Overview'!G20,'Steps Overview'!K20,'Steps Overview'!O20,'Steps Overview'!S20,'Steps Overview'!W20,'Steps Overview'!C34)</f>
-        <v>578.153846153846</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!C6,'Steps Overview'!G6,'Steps Overview'!K6,'Steps Overview'!O6,'Steps Overview'!S6,'Steps Overview'!W6,'Steps Overview'!C20,'Steps Overview'!G20,'Steps Overview'!K20,'Steps Overview'!O20,'Steps Overview'!S20,'Steps Overview'!W20,'Steps Overview'!C34)</f>
+        <v>133.553538461538</v>
       </c>
       <c r="D5" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!D6,'Steps Overview'!H6,'Steps Overview'!L6,'Steps Overview'!P6,'Steps Overview'!T6,'Steps Overview'!X6,'Steps Overview'!D20,'Steps Overview'!H20,'Steps Overview'!L20,'Steps Overview'!P20,'Steps Overview'!T20,'Steps Overview'!X20,'Steps Overview'!D34)</f>
-        <v>582.846153846154</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!D6,'Steps Overview'!H6,'Steps Overview'!L6,'Steps Overview'!P6,'Steps Overview'!T6,'Steps Overview'!X6,'Steps Overview'!D20,'Steps Overview'!H20,'Steps Overview'!L20,'Steps Overview'!P20,'Steps Overview'!T20,'Steps Overview'!X20,'Steps Overview'!D34)</f>
+        <v>134.637461538462</v>
       </c>
       <c r="E5" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!E6,'Steps Overview'!I6,'Steps Overview'!M6,'Steps Overview'!Q6,'Steps Overview'!U6,'Steps Overview'!Y6,'Steps Overview'!E20,'Steps Overview'!I20,'Steps Overview'!M20,'Steps Overview'!Q20,'Steps Overview'!U20,'Steps Overview'!Y20,'Steps Overview'!E34)</f>
-        <v>524.769230769231</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!E6,'Steps Overview'!I6,'Steps Overview'!M6,'Steps Overview'!Q6,'Steps Overview'!U6,'Steps Overview'!Y6,'Steps Overview'!E20,'Steps Overview'!I20,'Steps Overview'!M20,'Steps Overview'!Q20,'Steps Overview'!U20,'Steps Overview'!Y20,'Steps Overview'!E34)</f>
+        <v>121.221692307692</v>
       </c>
       <c r="F5" s="21" t="n">
         <f aca="false">C5-B5</f>
-        <v>-113</v>
+        <v>-26.103</v>
       </c>
       <c r="G5" s="21" t="n">
         <f aca="false">D5-C5</f>
-        <v>4.69230769230762</v>
+        <v>1.08392307692307</v>
       </c>
       <c r="H5" s="21" t="n">
         <f aca="false">E5-D5</f>
-        <v>-58.0769230769231</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>-13.4157692307692</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
         <f aca="false">results!A6</f>
         <v>LimitedGreedy</v>
       </c>
       <c r="B6" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B7,'Steps Overview'!F7,'Steps Overview'!J7,'Steps Overview'!N7,'Steps Overview'!R7,'Steps Overview'!V7,'Steps Overview'!B21,'Steps Overview'!F21,'Steps Overview'!J21,'Steps Overview'!N21,'Steps Overview'!R21,'Steps Overview'!V21,'Steps Overview'!B35)</f>
-        <v>519.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B7,'Steps Overview'!F7,'Steps Overview'!J7,'Steps Overview'!N7,'Steps Overview'!R7,'Steps Overview'!V7,'Steps Overview'!B21,'Steps Overview'!F21,'Steps Overview'!J21,'Steps Overview'!N21,'Steps Overview'!R21,'Steps Overview'!V21,'Steps Overview'!B35)</f>
+        <v>120.048923076923</v>
       </c>
       <c r="C6" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!C7,'Steps Overview'!G7,'Steps Overview'!K7,'Steps Overview'!O7,'Steps Overview'!S7,'Steps Overview'!W7,'Steps Overview'!C21,'Steps Overview'!G21,'Steps Overview'!K21,'Steps Overview'!O21,'Steps Overview'!S21,'Steps Overview'!W21,'Steps Overview'!C35)</f>
-        <v>519.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!C7,'Steps Overview'!G7,'Steps Overview'!K7,'Steps Overview'!O7,'Steps Overview'!S7,'Steps Overview'!W7,'Steps Overview'!C21,'Steps Overview'!G21,'Steps Overview'!K21,'Steps Overview'!O21,'Steps Overview'!S21,'Steps Overview'!W21,'Steps Overview'!C35)</f>
+        <v>120.048923076923</v>
       </c>
       <c r="D6" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!D7,'Steps Overview'!H7,'Steps Overview'!L7,'Steps Overview'!P7,'Steps Overview'!T7,'Steps Overview'!X7,'Steps Overview'!D21,'Steps Overview'!H21,'Steps Overview'!L21,'Steps Overview'!P21,'Steps Overview'!T21,'Steps Overview'!X21,'Steps Overview'!D35)</f>
-        <v>519.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!D7,'Steps Overview'!H7,'Steps Overview'!L7,'Steps Overview'!P7,'Steps Overview'!T7,'Steps Overview'!X7,'Steps Overview'!D21,'Steps Overview'!H21,'Steps Overview'!L21,'Steps Overview'!P21,'Steps Overview'!T21,'Steps Overview'!X21,'Steps Overview'!D35)</f>
+        <v>120.048923076923</v>
       </c>
       <c r="E6" s="20" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!E7,'Steps Overview'!I7,'Steps Overview'!M7,'Steps Overview'!Q7,'Steps Overview'!U7,'Steps Overview'!Y7,'Steps Overview'!E21,'Steps Overview'!I21,'Steps Overview'!M21,'Steps Overview'!Q21,'Steps Overview'!U21,'Steps Overview'!Y21,'Steps Overview'!E35)</f>
-        <v>519.692307692308</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!E7,'Steps Overview'!I7,'Steps Overview'!M7,'Steps Overview'!Q7,'Steps Overview'!U7,'Steps Overview'!Y7,'Steps Overview'!E21,'Steps Overview'!I21,'Steps Overview'!M21,'Steps Overview'!Q21,'Steps Overview'!U21,'Steps Overview'!Y21,'Steps Overview'!E35)</f>
+        <v>120.048923076923</v>
       </c>
       <c r="F6" s="21" t="n">
         <f aca="false">C6-B6</f>
@@ -9964,28 +9977,28 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10206,18 +10219,18 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5045045045045"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3873873873874"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.58108108108108"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>8</v>
@@ -10259,525 +10272,525 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">results!A2</f>
         <v>LimitedAStar</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B3:E3)</f>
-        <v>877.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B3:E3)</f>
+        <v>202.64475</v>
       </c>
       <c r="C2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F3:I3)</f>
-        <v>716</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F3:I3)</f>
+        <v>165.396</v>
       </c>
       <c r="D2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J3:M3)</f>
-        <v>628</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J3:M3)</f>
+        <v>145.068</v>
       </c>
       <c r="E2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N3:Q3)</f>
-        <v>514.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N3:Q3)</f>
+        <v>118.8495</v>
       </c>
       <c r="F2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R3:U3)</f>
-        <v>459.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R3:U3)</f>
+        <v>106.1445</v>
       </c>
       <c r="G2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V3:Y3)</f>
-        <v>447.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V3:Y3)</f>
+        <v>103.3725</v>
       </c>
       <c r="H2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B17:E17)</f>
-        <v>433</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B17:E17)</f>
+        <v>100.023</v>
       </c>
       <c r="I2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F17:I17)</f>
-        <v>439</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F17:I17)</f>
+        <v>101.409</v>
       </c>
       <c r="J2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J17:M17)</f>
-        <v>422.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J17:M17)</f>
+        <v>97.5975</v>
       </c>
       <c r="K2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N17:Q17)</f>
-        <v>427.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N17:Q17)</f>
+        <v>98.7525</v>
       </c>
       <c r="L2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R17:U17)</f>
-        <v>419</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R17:U17)</f>
+        <v>96.789</v>
       </c>
       <c r="M2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V17:Y17)</f>
-        <v>415</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V17:Y17)</f>
+        <v>95.865</v>
       </c>
       <c r="N2" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B31:E31)</f>
-        <v>412.75</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B31:E31)</f>
+        <v>95.34525</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">results!A3</f>
         <v>LimitedBestFirst</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B4:E4)</f>
-        <v>1027.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B4:E4)</f>
+        <v>237.29475</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F4:I4)</f>
-        <v>913</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F4:I4)</f>
+        <v>210.903</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J4:M4)</f>
-        <v>718.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J4:M4)</f>
+        <v>165.91575</v>
       </c>
       <c r="E3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N4:Q4)</f>
-        <v>586.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N4:Q4)</f>
+        <v>135.53925</v>
       </c>
       <c r="F3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R4:U4)</f>
-        <v>506</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R4:U4)</f>
+        <v>116.886</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V4:Y4)</f>
-        <v>490.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V4:Y4)</f>
+        <v>113.3055</v>
       </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B18:E18)</f>
-        <v>475</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B18:E18)</f>
+        <v>109.725</v>
       </c>
       <c r="I3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F18:I18)</f>
-        <v>467.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F18:I18)</f>
+        <v>107.9925</v>
       </c>
       <c r="J3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J18:M18)</f>
-        <v>463.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J18:M18)</f>
+        <v>107.0685</v>
       </c>
       <c r="K3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N18:Q18)</f>
-        <v>458.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N18:Q18)</f>
+        <v>105.97125</v>
       </c>
       <c r="L3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R18:U18)</f>
-        <v>455.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R18:U18)</f>
+        <v>105.16275</v>
       </c>
       <c r="M3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V18:Y18)</f>
-        <v>448</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V18:Y18)</f>
+        <v>103.488</v>
       </c>
       <c r="N3" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B32:E32)</f>
-        <v>441.5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B32:E32)</f>
+        <v>101.9865</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">results!A4</f>
         <v>LimitedBreadthFirstSearch</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B5:E5)</f>
-        <v>763.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B5:E5)</f>
+        <v>176.31075</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F5:I5)</f>
-        <v>741.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F5:I5)</f>
+        <v>171.2865</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J5:M5)</f>
-        <v>676.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J5:M5)</f>
+        <v>156.32925</v>
       </c>
       <c r="E4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N5:Q5)</f>
-        <v>486.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N5:Q5)</f>
+        <v>112.43925</v>
       </c>
       <c r="F4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R5:U5)</f>
-        <v>451</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R5:U5)</f>
+        <v>104.181</v>
       </c>
       <c r="G4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V5:Y5)</f>
-        <v>436.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V5:Y5)</f>
+        <v>100.77375</v>
       </c>
       <c r="H4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B19:E19)</f>
-        <v>429.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B19:E19)</f>
+        <v>99.27225</v>
       </c>
       <c r="I4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F19:I19)</f>
-        <v>425.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F19:I19)</f>
+        <v>98.34825</v>
       </c>
       <c r="J4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J19:M19)</f>
-        <v>422.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J19:M19)</f>
+        <v>97.53975</v>
       </c>
       <c r="K4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N19:Q19)</f>
-        <v>416.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N19:Q19)</f>
+        <v>96.15375</v>
       </c>
       <c r="L4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R19:U19)</f>
-        <v>415.75</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R19:U19)</f>
+        <v>96.03825</v>
       </c>
       <c r="M4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V19:Y19)</f>
-        <v>414</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V19:Y19)</f>
+        <v>95.634</v>
       </c>
       <c r="N4" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B33:E33)</f>
-        <v>411.75</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B33:E33)</f>
+        <v>95.11425</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
         <f aca="false">results!A5</f>
         <v>LimitedDijkstra</v>
       </c>
       <c r="B5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B6:E6)</f>
-        <v>958.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B6:E6)</f>
+        <v>221.4135</v>
       </c>
       <c r="C5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F6:I6)</f>
-        <v>747.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F6:I6)</f>
+        <v>172.6725</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J6:M6)</f>
-        <v>731.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J6:M6)</f>
+        <v>168.9765</v>
       </c>
       <c r="E5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N6:Q6)</f>
-        <v>699.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N6:Q6)</f>
+        <v>161.5845</v>
       </c>
       <c r="F5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R6:U6)</f>
-        <v>552.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R6:U6)</f>
+        <v>127.56975</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V6:Y6)</f>
-        <v>526</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V6:Y6)</f>
+        <v>121.506</v>
       </c>
       <c r="H5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B20:E20)</f>
-        <v>507</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B20:E20)</f>
+        <v>117.117</v>
       </c>
       <c r="I5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F20:I20)</f>
-        <v>512.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F20:I20)</f>
+        <v>118.3875</v>
       </c>
       <c r="J5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J20:M20)</f>
-        <v>508.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J20:M20)</f>
+        <v>117.4635</v>
       </c>
       <c r="K5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N20:Q20)</f>
-        <v>512.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N20:Q20)</f>
+        <v>118.32975</v>
       </c>
       <c r="L5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R20:U20)</f>
-        <v>487.25</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R20:U20)</f>
+        <v>112.55475</v>
       </c>
       <c r="M5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V20:Y20)</f>
-        <v>497.5</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V20:Y20)</f>
+        <v>114.9225</v>
       </c>
       <c r="N5" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B34:E34)</f>
-        <v>484.75</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B34:E34)</f>
+        <v>111.97725</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
         <f aca="false">results!A6</f>
         <v>LimitedGreedy</v>
       </c>
       <c r="B6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B7:E7)</f>
-        <v>907</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B7:E7)</f>
+        <v>209.517</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F7:I7)</f>
-        <v>624</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F7:I7)</f>
+        <v>144.144</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J7:M7)</f>
-        <v>659</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J7:M7)</f>
+        <v>152.229</v>
       </c>
       <c r="E6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N7:Q7)</f>
-        <v>517</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N7:Q7)</f>
+        <v>119.427</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R7:U7)</f>
-        <v>525</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R7:U7)</f>
+        <v>121.275</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V7:Y7)</f>
-        <v>486</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V7:Y7)</f>
+        <v>112.266</v>
       </c>
       <c r="H6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B21:E21)</f>
-        <v>438</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B21:E21)</f>
+        <v>101.178</v>
       </c>
       <c r="I6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F21:I21)</f>
-        <v>449</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F21:I21)</f>
+        <v>103.719</v>
       </c>
       <c r="J6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J21:M21)</f>
-        <v>439</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J21:M21)</f>
+        <v>101.409</v>
       </c>
       <c r="K6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N21:Q21)</f>
-        <v>430</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N21:Q21)</f>
+        <v>99.33</v>
       </c>
       <c r="L6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R21:U21)</f>
-        <v>435</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R21:U21)</f>
+        <v>100.485</v>
       </c>
       <c r="M6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V21:Y21)</f>
-        <v>425</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V21:Y21)</f>
+        <v>98.175</v>
       </c>
       <c r="N6" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B35:E35)</f>
-        <v>422</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B35:E35)</f>
+        <v>97.482</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="str">
         <f aca="false">results!A7</f>
         <v>UnlimitedAStarNonRecursive</v>
       </c>
       <c r="B7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B8:E8)</f>
-        <v>453</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B8:E8)</f>
+        <v>104.643</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F8:I8)</f>
-        <v>439</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F8:I8)</f>
+        <v>101.409</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J8:M8)</f>
-        <v>425</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J8:M8)</f>
+        <v>98.175</v>
       </c>
       <c r="E7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N8:Q8)</f>
-        <v>422</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N8:Q8)</f>
+        <v>97.482</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R8:U8)</f>
-        <v>415</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R8:U8)</f>
+        <v>95.865</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V8:Y8)</f>
-        <v>411</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V8:Y8)</f>
+        <v>94.941</v>
       </c>
       <c r="H7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B22:E22)</f>
-        <v>412</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B22:E22)</f>
+        <v>95.172</v>
       </c>
       <c r="I7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F22:I22)</f>
-        <v>411</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F22:I22)</f>
+        <v>94.941</v>
       </c>
       <c r="J7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J22:M22)</f>
-        <v>407</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J22:M22)</f>
+        <v>94.017</v>
       </c>
       <c r="K7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N22:Q22)</f>
-        <v>411</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N22:Q22)</f>
+        <v>94.941</v>
       </c>
       <c r="L7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R22:U22)</f>
-        <v>407</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R22:U22)</f>
+        <v>94.017</v>
       </c>
       <c r="M7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V22:Y22)</f>
-        <v>407</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V22:Y22)</f>
+        <v>94.017</v>
       </c>
       <c r="N7" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B36:E36)</f>
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B36:E36)</f>
+        <v>94.248</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
         <f aca="false">results!A8</f>
         <v>UnlimitedAStarRecursive</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B9:E9)</f>
-        <v>431</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B9:E9)</f>
+        <v>99.561</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F9:I9)</f>
-        <v>422</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F9:I9)</f>
+        <v>97.482</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J9:M9)</f>
-        <v>412</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J9:M9)</f>
+        <v>95.172</v>
       </c>
       <c r="E8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N9:Q9)</f>
-        <v>407</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N9:Q9)</f>
+        <v>94.017</v>
       </c>
       <c r="F8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R9:U9)</f>
-        <v>402</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R9:U9)</f>
+        <v>92.862</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V9:Y9)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V9:Y9)</f>
+        <v>92.631</v>
       </c>
       <c r="H8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B23:E23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B23:E23)</f>
+        <v>92.631</v>
       </c>
       <c r="I8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F23:I23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F23:I23)</f>
+        <v>92.631</v>
       </c>
       <c r="J8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J23:M23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J23:M23)</f>
+        <v>92.631</v>
       </c>
       <c r="K8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N23:Q23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N23:Q23)</f>
+        <v>92.631</v>
       </c>
       <c r="L8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R23:U23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R23:U23)</f>
+        <v>92.631</v>
       </c>
       <c r="M8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V23:Y23)</f>
-        <v>401</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V23:Y23)</f>
+        <v>92.631</v>
       </c>
       <c r="N8" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B37:E37)</f>
-        <v>401</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B37:E37)</f>
+        <v>92.631</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="str">
         <f aca="false">results!A9</f>
         <v>UnlimitedBestFirst</v>
       </c>
       <c r="B9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B10:E10)</f>
-        <v>487</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B10:E10)</f>
+        <v>112.497</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F10:I10)</f>
-        <v>494</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F10:I10)</f>
+        <v>114.114</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J10:M10)</f>
-        <v>493</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J10:M10)</f>
+        <v>113.883</v>
       </c>
       <c r="E9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N10:Q10)</f>
-        <v>484</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N10:Q10)</f>
+        <v>111.804</v>
       </c>
       <c r="F9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R10:U10)</f>
-        <v>464</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R10:U10)</f>
+        <v>107.184</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V10:Y10)</f>
-        <v>453</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V10:Y10)</f>
+        <v>104.643</v>
       </c>
       <c r="H9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B24:E24)</f>
-        <v>445</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B24:E24)</f>
+        <v>102.795</v>
       </c>
       <c r="I9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F24:I24)</f>
-        <v>440</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F24:I24)</f>
+        <v>101.64</v>
       </c>
       <c r="J9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J24:M24)</f>
-        <v>436</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J24:M24)</f>
+        <v>100.716</v>
       </c>
       <c r="K9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N24:Q24)</f>
-        <v>433</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N24:Q24)</f>
+        <v>100.023</v>
       </c>
       <c r="L9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R24:U24)</f>
-        <v>427</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R24:U24)</f>
+        <v>98.637</v>
       </c>
       <c r="M9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V24:Y24)</f>
-        <v>421</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V24:Y24)</f>
+        <v>97.251</v>
       </c>
       <c r="N9" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B38:E38)</f>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B38:E38)</f>
+        <v>97.02</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">results!A10</f>
         <v>UnlimitedBreadthFirstSearch</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B11:E11)</f>
-        <v>424</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B11:E11)</f>
+        <v>97.944</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F11:I11)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F11:I11)</f>
         <v>0</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J11:M11)</f>
-        <v>407</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J11:M11)</f>
+        <v>94.017</v>
       </c>
       <c r="E10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N11:Q11)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N11:Q11)</f>
         <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R11:U11)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R11:U11)</f>
         <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V11:Y11)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V11:Y11)</f>
         <v>0</v>
       </c>
       <c r="H10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B25:E25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B25:E25)</f>
         <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F25:I25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F25:I25)</f>
         <v>0</v>
       </c>
       <c r="J10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J25:M25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J25:M25)</f>
         <v>0</v>
       </c>
       <c r="K10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N25:Q25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N25:Q25)</f>
         <v>0</v>
       </c>
       <c r="L10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R25:U25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R25:U25)</f>
         <v>0</v>
       </c>
       <c r="M10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V25:Y25)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V25:Y25)</f>
         <v>0</v>
       </c>
       <c r="N10" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B39:E39)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B39:E39)</f>
         <v>0</v>
       </c>
     </row>
@@ -10787,56 +10800,56 @@
         <v>UnlimitedGreedy</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B12:E12)</f>
-        <v>907</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B12:E12)</f>
+        <v>209.517</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F12:I12)</f>
-        <v>624</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F12:I12)</f>
+        <v>144.144</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J12:M12)</f>
-        <v>659</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J12:M12)</f>
+        <v>152.229</v>
       </c>
       <c r="E11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N12:Q12)</f>
-        <v>517</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N12:Q12)</f>
+        <v>119.427</v>
       </c>
       <c r="F11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R12:U12)</f>
-        <v>525</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R12:U12)</f>
+        <v>121.275</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V12:Y12)</f>
-        <v>486</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V12:Y12)</f>
+        <v>112.266</v>
       </c>
       <c r="H11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B26:E26)</f>
-        <v>438</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B26:E26)</f>
+        <v>101.178</v>
       </c>
       <c r="I11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F26:I26)</f>
-        <v>449</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F26:I26)</f>
+        <v>103.719</v>
       </c>
       <c r="J11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J26:M26)</f>
-        <v>439</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J26:M26)</f>
+        <v>101.409</v>
       </c>
       <c r="K11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N26:Q26)</f>
-        <v>430</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N26:Q26)</f>
+        <v>99.33</v>
       </c>
       <c r="L11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R26:U26)</f>
-        <v>435</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R26:U26)</f>
+        <v>100.485</v>
       </c>
       <c r="M11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V26:Y26)</f>
-        <v>425</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V26:Y26)</f>
+        <v>98.175</v>
       </c>
       <c r="N11" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B40:E40)</f>
-        <v>422</v>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B40:E40)</f>
+        <v>97.482</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10845,61 +10858,61 @@
         <v>0</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B13:E13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B13:E13)</f>
         <v>0</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F13:I13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F13:I13)</f>
         <v>0</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J13:M13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J13:M13)</f>
         <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N13:Q13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N13:Q13)</f>
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R13:U13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R13:U13)</f>
         <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V13:Y13)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V13:Y13)</f>
         <v>0</v>
       </c>
       <c r="H12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B27:E27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B27:E27)</f>
         <v>0</v>
       </c>
       <c r="I12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!F27:I27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!F27:I27)</f>
         <v>0</v>
       </c>
       <c r="J12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!J27:M27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!J27:M27)</f>
         <v>0</v>
       </c>
       <c r="K12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!N27:Q27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!N27:Q27)</f>
         <v>0</v>
       </c>
       <c r="L12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!R27:U27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!R27:U27)</f>
         <v>0</v>
       </c>
       <c r="M12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!V27:Y27)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!V27:Y27)</f>
         <v>0</v>
       </c>
       <c r="N12" s="0" t="n">
-        <f aca="false">AVERAGE('Steps Overview'!B41:E41)</f>
+        <f aca="false">0.231*AVERAGE('Steps Overview'!B41:E41)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>8</v>
@@ -11581,7 +11594,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B25" s="3" t="n">
         <v>8</v>
@@ -11630,55 +11643,55 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B2/B14</f>
-        <v>0.0396004965579506</v>
+        <v>0.00914771470488658</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C2/C14</f>
-        <v>0.0157602504911321</v>
+        <v>0.00364061786345152</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">D2/D14</f>
-        <v>0.0221506988228032</v>
+        <v>0.00511681142806755</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">E2/E14</f>
-        <v>0.0204176794483853</v>
+        <v>0.00471648395257701</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">F2/F14</f>
-        <v>0.016532939948908</v>
+        <v>0.00381910912819775</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">G2/G14</f>
-        <v>0.0165829797483834</v>
+        <v>0.00383066832187656</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">H2/H14</f>
-        <v>0.012990324758119</v>
+        <v>0.00300076501912548</v>
       </c>
       <c r="I26" s="0" t="n">
         <f aca="false">I2/I14</f>
-        <v>0.0137304423297965</v>
+        <v>0.00317173217818298</v>
       </c>
       <c r="J26" s="0" t="n">
         <f aca="false">J2/J14</f>
-        <v>0.0131698916016614</v>
+        <v>0.00304224495998379</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">K2/K14</f>
-        <v>0.0118494906797866</v>
+        <v>0.0027372323470307</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">L2/L14</f>
-        <v>0.0119894984583909</v>
+        <v>0.00276957414388829</v>
       </c>
       <c r="M26" s="0" t="n">
         <f aca="false">M2/M14</f>
-        <v>0.0110753054048825</v>
+        <v>0.00255839554852785</v>
       </c>
       <c r="N26" s="0" t="n">
         <f aca="false">N2/N14</f>
-        <v>0.0107282332529745</v>
+        <v>0.0024782218814371</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11688,55 +11701,55 @@
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">B3/B15</f>
-        <v>0.0341111913597158</v>
+        <v>0.00787968520409434</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C3/C15</f>
-        <v>0.0265545925193415</v>
+        <v>0.00613411087196789</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">D3/D15</f>
-        <v>0.0316141597984088</v>
+        <v>0.00730287091343244</v>
       </c>
       <c r="E27" s="0" t="n">
         <f aca="false">E3/E15</f>
-        <v>0.0251405923624873</v>
+        <v>0.00580747683573456</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">F3/F15</f>
-        <v>0.0230232849131508</v>
+        <v>0.00531837881493784</v>
       </c>
       <c r="G27" s="0" t="n">
         <f aca="false">G3/G15</f>
-        <v>0.0206778803591754</v>
+        <v>0.00477659036296952</v>
       </c>
       <c r="H27" s="0" t="n">
         <f aca="false">H3/H15</f>
-        <v>0.0198957046220863</v>
+        <v>0.00459590776770194</v>
       </c>
       <c r="I27" s="0" t="n">
         <f aca="false">I3/I15</f>
-        <v>0.018808146844355</v>
+        <v>0.00434468192104602</v>
       </c>
       <c r="J27" s="0" t="n">
         <f aca="false">J3/J15</f>
-        <v>0.0159735325286257</v>
+        <v>0.00368988601411254</v>
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">K3/K15</f>
-        <v>0.0154424883024203</v>
+        <v>0.00356721479785909</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">L3/L15</f>
-        <v>0.0169700019570019</v>
+        <v>0.00392007045206743</v>
       </c>
       <c r="M27" s="0" t="n">
         <f aca="false">M3/M15</f>
-        <v>0.0172784511102755</v>
+        <v>0.00399132220647363</v>
       </c>
       <c r="N27" s="0" t="n">
         <f aca="false">N3/N15</f>
-        <v>0.0154695164681149</v>
+        <v>0.00357345830413455</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11746,55 +11759,55 @@
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">B4/B16</f>
-        <v>0.0549456482614643</v>
+        <v>0.0126924447483982</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C4/C16</f>
-        <v>0.0278835396865687</v>
+        <v>0.00644109766759737</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">D4/D16</f>
-        <v>0.0485900450539391</v>
+        <v>0.0112243004074599</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">E4/E16</f>
-        <v>0.0368736032726033</v>
+        <v>0.00851780235597136</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">F4/F16</f>
-        <v>0.0496013197690404</v>
+        <v>0.0114579048666483</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">G4/G16</f>
-        <v>0.0378024739498711</v>
+        <v>0.00873237148242023</v>
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">H4/H16</f>
-        <v>0.0419442207744675</v>
+        <v>0.00968911499890198</v>
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">I4/I16</f>
-        <v>0.0320257258913796</v>
+        <v>0.00739794268090868</v>
       </c>
       <c r="J28" s="0" t="n">
         <f aca="false">J4/J16</f>
-        <v>0.0327560460019782</v>
+        <v>0.00756664662645696</v>
       </c>
       <c r="K28" s="0" t="n">
         <f aca="false">K4/K16</f>
-        <v>0.0601083032490975</v>
+        <v>0.0138850180505415</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">L4/L16</f>
-        <v>0.0755051078320091</v>
+        <v>0.0174416799091941</v>
       </c>
       <c r="M28" s="0" t="n">
         <f aca="false">M4/M16</f>
-        <v>0.160776699029126</v>
+        <v>0.0371394174757282</v>
       </c>
       <c r="N28" s="0" t="n">
         <f aca="false">N4/N16</f>
-        <v>0.156499429874572</v>
+        <v>0.0361513683010262</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11804,55 +11817,55 @@
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B5/B17</f>
-        <v>0.117283572958091</v>
+        <v>0.0270925053533191</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C5/C17</f>
-        <v>0.19217173340189</v>
+        <v>0.0443916704158365</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">D5/D17</f>
-        <v>0.135960224896613</v>
+        <v>0.0314068119511175</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">E5/E17</f>
-        <v>0.135831836496917</v>
+        <v>0.0313771542307879</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">F5/F17</f>
-        <v>0.157538154328912</v>
+        <v>0.0363913136499786</v>
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">G5/G17</f>
-        <v>0.149900256483329</v>
+        <v>0.0346269592476489</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">H5/H17</f>
-        <v>0.148223943867856</v>
+        <v>0.0342397310334746</v>
       </c>
       <c r="I29" s="0" t="n">
         <f aca="false">I5/I17</f>
-        <v>0.154728658766699</v>
+        <v>0.0357423201751076</v>
       </c>
       <c r="J29" s="0" t="n">
         <f aca="false">J5/J17</f>
-        <v>0.152234114213008</v>
+        <v>0.0351660803832049</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">K5/K17</f>
-        <v>0.151028230264613</v>
+        <v>0.0348875211911255</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">L5/L17</f>
-        <v>0.145491191400418</v>
+        <v>0.0336084652134966</v>
       </c>
       <c r="M29" s="0" t="n">
         <f aca="false">M5/M17</f>
-        <v>0.144927536231884</v>
+        <v>0.0334782608695652</v>
       </c>
       <c r="N29" s="0" t="n">
         <f aca="false">N5/N17</f>
-        <v>0.142113749633539</v>
+        <v>0.0328282761653474</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11862,55 +11875,55 @@
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">B6/B18</f>
-        <v>27.9076923076923</v>
+        <v>6.44667692307692</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C6/C18</f>
-        <v>69.3333333333333</v>
+        <v>16.016</v>
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">D6/D18</f>
-        <v>50.6923076923077</v>
+        <v>11.7099230769231</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">E6/E18</f>
-        <v>103.4</v>
+        <v>23.8854</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">F6/F18</f>
-        <v>95.4545454545455</v>
+        <v>22.05</v>
       </c>
       <c r="G30" s="0" t="n">
         <f aca="false">G6/G18</f>
-        <v>121.5</v>
+        <v>28.0665</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">H6/H18</f>
-        <v>146</v>
+        <v>33.726</v>
       </c>
       <c r="I30" s="0" t="n">
         <f aca="false">I6/I18</f>
-        <v>149.666666666667</v>
+        <v>34.573</v>
       </c>
       <c r="J30" s="0" t="n">
         <f aca="false">J6/J18</f>
-        <v>146.333333333333</v>
+        <v>33.803</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">K6/K18</f>
-        <v>172</v>
+        <v>39.732</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">L6/L18</f>
-        <v>145</v>
+        <v>33.495</v>
       </c>
       <c r="M30" s="0" t="n">
         <f aca="false">M6/M18</f>
-        <v>154.545454545455</v>
+        <v>35.7</v>
       </c>
       <c r="N30" s="0" t="n">
         <f aca="false">N6/N18</f>
-        <v>211</v>
+        <v>48.741</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11920,55 +11933,55 @@
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B7/B19</f>
-        <v>0.00212050606602825</v>
+        <v>0.000489836901252526</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C7/C19</f>
-        <v>0.00364798218388656</v>
+        <v>0.000842683884477794</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">D7/D19</f>
-        <v>0.00608653622384132</v>
+        <v>0.00140598986770735</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">E7/E19</f>
-        <v>0.00712958269978037</v>
+        <v>0.00164693360364927</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">F7/F19</f>
-        <v>0.0102725314983044</v>
+        <v>0.00237295477610832</v>
       </c>
       <c r="G31" s="0" t="n">
         <f aca="false">G7/G19</f>
-        <v>0.0139552650566614</v>
+        <v>0.00322366622808879</v>
       </c>
       <c r="H31" s="0" t="n">
         <f aca="false">H7/H19</f>
-        <v>0.013535378423884</v>
+        <v>0.00312667241591721</v>
       </c>
       <c r="I31" s="0" t="n">
         <f aca="false">I7/I19</f>
-        <v>0.0211131944622814</v>
+        <v>0.00487714792078699</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false">J7/J19</f>
-        <v>0.0358669310420798</v>
+        <v>0.00828526107072043</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">K7/K19</f>
-        <v>0.0282362640193738</v>
+        <v>0.00652257698847535</v>
       </c>
       <c r="L31" s="0" t="n">
         <f aca="false">L7/L19</f>
-        <v>0.0306990250985273</v>
+        <v>0.0070914747977598</v>
       </c>
       <c r="M31" s="0" t="n">
         <f aca="false">M7/M19</f>
-        <v>0.0548572968965866</v>
+        <v>0.0126720355831115</v>
       </c>
       <c r="N31" s="0" t="n">
         <f aca="false">N7/N19</f>
-        <v>0.0450331125827815</v>
+        <v>0.0104026490066225</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11978,55 +11991,55 @@
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">B8/B20</f>
-        <v>0.0150333978618392</v>
+        <v>0.00347271490608486</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C8/C20</f>
-        <v>0.0208580466587584</v>
+        <v>0.00481820877817319</v>
       </c>
       <c r="D32" s="0" t="n">
         <f aca="false">D8/D20</f>
-        <v>0.0395621279047436</v>
+        <v>0.00913885154599578</v>
       </c>
       <c r="E32" s="0" t="n">
         <f aca="false">E8/E20</f>
-        <v>0.0698203027833769</v>
+        <v>0.0161284899429601</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">F8/F20</f>
-        <v>0.221670802315964</v>
+        <v>0.0512059553349876</v>
       </c>
       <c r="G32" s="0" t="n">
         <f aca="false">G8/G20</f>
-        <v>0.198024691358025</v>
+        <v>0.0457437037037037</v>
       </c>
       <c r="H32" s="0" t="n">
         <f aca="false">H8/H20</f>
-        <v>0.65469387755102</v>
+        <v>0.151234285714286</v>
       </c>
       <c r="I32" s="0" t="n">
         <f aca="false">I8/I20</f>
-        <v>1.12640449438202</v>
+        <v>0.260199438202247</v>
       </c>
       <c r="J32" s="0" t="n">
         <f aca="false">J8/J20</f>
-        <v>0.916047972587093</v>
+        <v>0.211607081667618</v>
       </c>
       <c r="K32" s="0" t="n">
         <f aca="false">K8/K20</f>
-        <v>0.792881858625803</v>
+        <v>0.183155709342561</v>
       </c>
       <c r="L32" s="0" t="n">
         <f aca="false">L8/L20</f>
-        <v>0.904171364148816</v>
+        <v>0.208863585118377</v>
       </c>
       <c r="M32" s="0" t="n">
         <f aca="false">M8/M20</f>
-        <v>0.860053619302949</v>
+        <v>0.198672386058981</v>
       </c>
       <c r="N32" s="0" t="n">
         <f aca="false">N8/N20</f>
-        <v>0.774131274131274</v>
+        <v>0.178824324324324</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12036,55 +12049,55 @@
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">B9/B21</f>
-        <v>10.6448087431694</v>
+        <v>2.45895081967213</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C9/C21</f>
-        <v>10.4550264550265</v>
+        <v>2.41511111111111</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">D9/D21</f>
-        <v>10.2708333333333</v>
+        <v>2.3725625</v>
       </c>
       <c r="E33" s="0" t="n">
         <f aca="false">E9/E21</f>
-        <v>26.8888888888889</v>
+        <v>6.21133333333333</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">F9/F21</f>
-        <v>27.2941176470588</v>
+        <v>6.30494117647059</v>
       </c>
       <c r="G33" s="0" t="n">
         <f aca="false">G9/G21</f>
-        <v>28.3125</v>
+        <v>6.5401875</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">H9/H21</f>
-        <v>27.8125</v>
+        <v>6.4246875</v>
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">I9/I21</f>
-        <v>27.5</v>
+        <v>6.3525</v>
       </c>
       <c r="J33" s="0" t="n">
         <f aca="false">J9/J21</f>
-        <v>27.25</v>
+        <v>6.29475</v>
       </c>
       <c r="K33" s="0" t="n">
         <f aca="false">K9/K21</f>
-        <v>27.0625</v>
+        <v>6.2514375</v>
       </c>
       <c r="L33" s="0" t="n">
         <f aca="false">L9/L21</f>
-        <v>26.6875</v>
+        <v>6.1648125</v>
       </c>
       <c r="M33" s="0" t="n">
         <f aca="false">M9/M21</f>
-        <v>27.6065573770492</v>
+        <v>6.37711475409836</v>
       </c>
       <c r="N33" s="0" t="n">
         <f aca="false">N9/N21</f>
-        <v>28</v>
+        <v>6.468</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12094,7 +12107,7 @@
       </c>
       <c r="B34" s="0" t="n">
         <f aca="false">B10/B22</f>
-        <v>0.000424000424000424</v>
+        <v>9.7944097944098E-005</v>
       </c>
       <c r="C34" s="0" t="e">
         <f aca="false">C10/C22</f>
@@ -12102,7 +12115,7 @@
       </c>
       <c r="D34" s="0" t="n">
         <f aca="false">D10/D22</f>
-        <v>0.000407000407000407</v>
+        <v>9.4017094017094E-005</v>
       </c>
       <c r="E34" s="0" t="e">
         <f aca="false">E10/E22</f>
@@ -12152,55 +12165,55 @@
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B11/B23</f>
-        <v>27.2781954887218</v>
+        <v>6.30126315789474</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C11/C23</f>
-        <v>62.4</v>
+        <v>14.4144</v>
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">D11/D23</f>
-        <v>47.0714285714286</v>
+        <v>10.8735</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">E11/E23</f>
-        <v>86.1666666666667</v>
+        <v>19.9045</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">F11/F23</f>
-        <v>87.5</v>
+        <v>20.2125</v>
       </c>
       <c r="G35" s="0" t="n">
         <f aca="false">G11/G23</f>
-        <v>108</v>
+        <v>24.948</v>
       </c>
       <c r="H35" s="0" t="n">
         <f aca="false">H11/H23</f>
-        <v>146</v>
+        <v>33.726</v>
       </c>
       <c r="I35" s="0" t="n">
         <f aca="false">I11/I23</f>
-        <v>74.8333333333333</v>
+        <v>17.2865</v>
       </c>
       <c r="J35" s="0" t="n">
         <f aca="false">J11/J23</f>
-        <v>146.333333333333</v>
+        <v>33.803</v>
       </c>
       <c r="K35" s="0" t="n">
         <f aca="false">K11/K23</f>
-        <v>143.333333333333</v>
+        <v>33.11</v>
       </c>
       <c r="L35" s="0" t="n">
         <f aca="false">L11/L23</f>
-        <v>145</v>
+        <v>33.495</v>
       </c>
       <c r="M35" s="0" t="n">
         <f aca="false">M11/M23</f>
-        <v>141.666666666667</v>
+        <v>32.725</v>
       </c>
       <c r="N35" s="0" t="n">
         <f aca="false">N11/N23</f>
-        <v>168.8</v>
+        <v>38.9928</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12274,33 +12287,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:N36">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.1"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF00CC00"/>
-      </colorScale>
+  <conditionalFormatting sqref="B2:N36">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:N12">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="num" val="400"/>
-        <cfvo type="num" val="450"/>
-        <cfvo type="num" val="1000"/>
+        <cfvo type="num" val="90"/>
+        <cfvo type="num" val="115"/>
+        <cfvo type="num" val="250"/>
         <color rgb="FF00CC00"/>
         <color rgb="FFFFFF00"/>
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:N36">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
+  <conditionalFormatting sqref="B26:N36">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.025"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00CC00"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -12320,7 +12333,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>